<commit_message>
Database Updated, Update Database.py added to menu
</commit_message>
<xml_diff>
--- a/Datos/Database by set/Set by name/Xlsx sets/Kaldheim (KHM).xlsx
+++ b/Datos/Database by set/Set by name/Xlsx sets/Kaldheim (KHM).xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A264"/>
+  <dimension ref="A1:A293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,14 +458,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Alpine Meadow</t>
+          <t>Aegar, the Freezing Flame</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Alrund, God of the Cosmos // Hakka, Whispering Raven</t>
+          <t>Alpine Meadow</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Alrund's Epiphany</t>
+          <t>Alrund, God of the Cosmos // Hakka, Whispering Raven</t>
         </is>
       </c>
     </row>
@@ -493,1790 +493,1993 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Annul</t>
+          <t>Alrund's Epiphany</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Arctic Treeline</t>
+          <t>Annul</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Armed and Armored</t>
+          <t>Arctic Treeline</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Augury Raven</t>
+          <t>Armed and Armored</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Axgard Cavalry</t>
+          <t>Arni Slays the Troll</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Axguard Armory</t>
+          <t>Ascendant Spirit</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Barkchannel Pathway // Tidechannel Pathway</t>
+          <t>Augury Raven</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Barkchannel Pathway // Tidechannel Pathway</t>
+          <t>Avalanche Caller</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Basalt Ravager</t>
+          <t>Axgard Armory</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Battle for Bretagard</t>
+          <t>Axgard Braggart</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Battle of Frost and Fire</t>
+          <t>Axgard Cavalry</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Bearded Axe</t>
+          <t>Barkchannel Pathway // Tidechannel Pathway</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>"Beasts of Littjara"</t>
+          <t>Barkchannel Pathway // Tidechannel Pathway</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Behold the Multiverse</t>
+          <t>Basalt Ravager</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>"Big-Booty Ox"</t>
+          <t>Battle for Bretagard</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Binding the Old Gods</t>
+          <t>Battle of Frost and Fire</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Blightstep Pathway // Searstep Pathway</t>
+          <t>Bearded Axe</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Blightstep Pathway // Searstep Pathway</t>
+          <t>Behold the Multiverse</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Blizzard Brawl</t>
+          <t>Berg Strider</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Bloodline Pretender</t>
+          <t>Beskir Shieldmate</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Bloodsky Berserker</t>
+          <t>Binding the Old Gods</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Boreal Outrider</t>
+          <t>Blightstep Pathway // Searstep Pathway</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Bound in Gold</t>
+          <t>Blightstep Pathway // Searstep Pathway</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>"Breakneck Berserker"</t>
+          <t>Blizzard Brawl</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bretagard Stronghold</t>
+          <t>Bloodline Pretender</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Broken Wings</t>
+          <t>Bloodsky Berserker</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Burning-Rune Demon</t>
+          <t>Boreal Outrider</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Calamity Bearer</t>
+          <t>Bound in Gold</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Calamity Bearer</t>
+          <t>"Breakneck Berserker"</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Canopy Tactician</t>
+          <t>Bretagard Stronghold</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Cinderheart Giant</t>
+          <t>Broken Wings</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Clarion Spirit</t>
+          <t>Burning-Rune Demon</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Cleaving Reaper</t>
+          <t>Calamity Bearer</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Codespell Cleric</t>
+          <t>Calamity Bearer</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Cosmos Charger</t>
+          <t>Canopy Tactician</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Cosmos Charger</t>
+          <t>Cinderheart Giant</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Crush the Weak</t>
+          <t>Clarion Spirit</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>"Cyclone Summoner"</t>
+          <t>Cleaving Reaper</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>"Cyclone Summoner"</t>
+          <t>Codespell Cleric</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Darkbore Pathway // Slitherbore Pathway</t>
+          <t>Cosima, God of the Voyage // The Omenkeel</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Darkbore Pathway // Slitherbore Pathway</t>
+          <t>Cosima, God of the Voyage // The Omenkeel</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Deathknell Berserker</t>
+          <t>Cosmos Charger</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>"Demonic Lightning"</t>
+          <t>Cosmos Charger</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Divine Gambit</t>
+          <t>Crush the Weak</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Dogged Pursuit</t>
+          <t>Cyclone Summoner</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Doomskar Oracle</t>
+          <t>Cyclone Summoner</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>"Dragon Dad uwu…"</t>
+          <t>Darkbore Pathway // Slitherbore Pathway</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Draugr Necromancer</t>
+          <t>Darkbore Pathway // Slitherbore Pathway</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Draugr Necromancer</t>
+          <t>Deathknell Berserker</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>"Draugr Omenreader"</t>
+          <t>"Demonic Lightning"</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Draugr's Helm</t>
+          <t>Divine Gambit</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Dual Strike</t>
+          <t>Dogged Pursuit</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Duskwielder</t>
+          <t>Doomskar Oracle</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Egon, God of Death // Throne of Death</t>
+          <t>"Dragon Dad uwu…"</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Egon, God of Death // Throne of Death</t>
+          <t>Draugr Necromancer</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Elderfang Disciple</t>
+          <t>Draugr Necromancer</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Elderfang Ritualist</t>
+          <t>Draugr's Helm</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Elderleaf Mentor</t>
+          <t>Dread Rider</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Elven Ambush</t>
+          <t>Dual Strike</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Elvish Warmaster</t>
+          <t>Duskwielder</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Elvish Warmaster</t>
+          <t>Dwarven Reinforcements</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Eradicator Valkyrie</t>
+          <t>Egon, God of Death // Throne of Death</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Eradicator Valkyrie</t>
+          <t>Egon, God of Death // Throne of Death</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Esika, God of the Tree // The Prismatic Bridge</t>
+          <t>Elderfang Disciple</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Esika, God of the Tree // The Prismatic Bridge</t>
+          <t>Elderfang Ritualist</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Esika's Chariot</t>
+          <t>Elderleaf Mentor</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Esika's Chariot</t>
+          <t>Elven Ambush</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Faceless Haven</t>
+          <t>Elvish Warmaster</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Faceless Haven</t>
+          <t>Elvish Warmaster</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Feed the Serpent</t>
+          <t>Eradicator Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Fire Giant's Fury</t>
+          <t>Eradicator Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Firja, Judge of Valor</t>
+          <t>Esika, God of the Tree // The Prismatic Bridge</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Firja, Judge of Valor</t>
+          <t>Esika, God of the Tree // The Prismatic Bridge</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Firja's Judgment</t>
+          <t>Esika's Chariot</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Forest</t>
+          <t>Esika's Chariot</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Forging the Tyrite Sword</t>
+          <t>Faceless Haven</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>"Frigid-Sea Traveler"</t>
+          <t>Faceless Haven</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Frost Bite</t>
+          <t>Fall of the Impostor</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Frost Bite</t>
+          <t>Fearless Liberator</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Frostpeak Yeti</t>
+          <t>Feed the Serpent</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Frostpyre Arcanist</t>
+          <t>Fire Giant's Fury</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Funeral Longboat</t>
+          <t>Firja, Judge of Valor</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Giant's Amulet</t>
+          <t>Firja, Judge of Valor</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Giant's Grasp</t>
+          <t>Firja's Retribution</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Gilded Assault Cart</t>
+          <t>Forest</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Glacial Floodplain</t>
+          <t>Forging the Tyrite Sword</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Gladewalker Ritualist</t>
+          <t>Frost Bite</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Glimpse the Cosmos</t>
+          <t>Frost Bite</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Glittering Frost</t>
+          <t>Frostpeak Yeti</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Gnottvold Recluse</t>
+          <t>Frostpyre Arcanist</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Gods' Hall Guardian</t>
+          <t>Funeral Longboat</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Goldspan Dragon</t>
+          <t>Gates of Istfell</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Goldspan Dragon</t>
+          <t>Giant Ox</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Goldvein Pick</t>
+          <t>Giant's Amulet</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Grim Draugr</t>
+          <t>Giant's Grasp</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Guardian Gladewalker</t>
+          <t>Gilded Assault Cart</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Hagi Mob</t>
+          <t>Glacial Floodplain</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Hailstorm Valkyrie</t>
+          <t>Gladewalker Ritualist</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Halvar, God of Battle // Sword of the Realms</t>
+          <t>Glimpse the Cosmos</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Halvar, God of Battle // Sword of the Realms</t>
+          <t>Glittering Frost</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Harald, King of Skemfar</t>
+          <t>Gnottvold Recluse</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Harald, King of Skemfar</t>
+          <t>Gnottvold Slumbermound</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Harald Unites the Elves</t>
+          <t>Gods' Hall Guardian</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Hengegate Pathway // Mistgate Pathway</t>
+          <t>Goldmaw Champion</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Hengegate Pathway // Mistgate Pathway</t>
+          <t>Goldspan Dragon</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Highland Forest</t>
+          <t>Goldspan Dragon</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Ice Tunnel</t>
+          <t>Goldvein Pick</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Infernal Pet</t>
+          <t>Grim Draugr</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Inga Rune-Eyes</t>
+          <t>Guardian Gladewalker</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Inga Rune-Eyes</t>
+          <t>Hagi Mob</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Invasion of the Giants</t>
+          <t>Hailstorm Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Iron Verdict</t>
+          <t>Halvar, God of Battle // Sword of the Realms</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Island</t>
+          <t>Halvar, God of Battle // Sword of the Realms</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>"Jack and Jill Storm the Hill"</t>
+          <t>Harald, King of Skemfar</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Jaspera Sentinel</t>
+          <t>Harald, King of Skemfar</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
+          <t>Harald Unites the Elves</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
+          <t>Hengegate Pathway // Mistgate Pathway</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Kardur, Doomscourge</t>
+          <t>Hengegate Pathway // Mistgate Pathway</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Kardur, Doomscourge</t>
+          <t>Highland Forest</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Kardur's Vicious Return</t>
+          <t>Ice Tunnel</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Karfell Kennel-Master</t>
+          <t>Infernal Pet</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Kaya's Onslaught</t>
+          <t>Inga Rune-Eyes</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Kaya the Inexorable</t>
+          <t>Inga Rune-Eyes</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Kaya the Inexorable</t>
+          <t>Invasion of the Giants</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>King Harald's Revenge</t>
+          <t>Iron Verdict</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Koll, the Forgemaster</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Koll, the Forgemaster</t>
+          <t>Jaspera Sentinel</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
+          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
+          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Koma, Cosmos Serpent</t>
+          <t>Kardur, Doomscourge</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Koma, Cosmos Serpent</t>
+          <t>Kardur, Doomscourge</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Koma's Faithful</t>
+          <t>Kardur's Vicious Return</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Littjara Kinseekers</t>
+          <t>Karfell Harbinger</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Magda, Brazen Outlaw</t>
+          <t>Karfell Kennel-Master</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Magda, Brazen Outlaw</t>
+          <t>Kaya's Onslaught</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Mammoth Growth</t>
+          <t>Kaya the Inexorable</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Masked Vandal</t>
+          <t>Kaya the Inexorable</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Masked Vandal</t>
+          <t>King Harald's Revenge</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Maskwood Nexus</t>
+          <t>Koll, the Forgemaster</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Maskwood Nexus</t>
+          <t>Koll, the Forgemaster</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Moritte of the Frost</t>
+          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Mountain</t>
+          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>"My Larger Pony"</t>
+          <t>Koma, Cosmos Serpent</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>"Mystic Reflection"</t>
+          <t>Koma, Cosmos Serpent</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Narfi, Betrayer King</t>
+          <t>Koma's Faithful</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Niko Aris</t>
+          <t>Littjara Kinseekers</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Niko Aris</t>
+          <t>Magda, Brazen Outlaw</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Old-Growth Troll</t>
+          <t>Magda, Brazen Outlaw</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Old-Growth Troll</t>
+          <t>Mammoth Growth</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Open the Omenpaths</t>
+          <t>Masked Vandal</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Path to the World Tree</t>
+          <t>Masked Vandal</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Plains</t>
+          <t>Maskwood Nexus</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Pyre of Heroes</t>
+          <t>Maskwood Nexus</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Pyre of Heroes</t>
+          <t>Moritte of the Frost</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Quakebringer</t>
+          <t>Mountain</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Quakebringer</t>
+          <t>Mystic Reflection</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>"Raiding Karve"</t>
+          <t>Mystic Reflection</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Raise the Draugr</t>
+          <t>Narfi, Betrayer King</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Rally the Ranks</t>
+          <t>Narfi, Betrayer King</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Rally the Ranks</t>
+          <t>Niko Aris</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Rampage of the Valkyries</t>
+          <t>Niko Aris</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Ravenform</t>
+          <t>Niko Defies Destiny</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Old-Growth Troll</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Old-Growth Troll</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Open the Omenpaths</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Reckless Crew</t>
+          <t>Path to the World Tree</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Reckless Crew</t>
+          <t>Pilfering Hawk</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Plains</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Poison the Cup</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Pyre of Heroes</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>"Reidane, God of Justice" // "Reidane's Shield"</t>
+          <t>Pyre of Heroes</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>"Reidane, God of Justice" // "Reidane's Shield"</t>
+          <t>Quakebringer</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Renegade Reaper</t>
+          <t>Quakebringer</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Replicating Ring</t>
+          <t>Raiders' Karve</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>"Resolute Valkyrie"</t>
+          <t>Raise the Draugr</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Rimewood Falls</t>
+          <t>Rally the Ranks</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Rise of the Dread Marn</t>
+          <t>Rally the Ranks</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Rise of the Dread Marn</t>
+          <t>Rampage of the Valkyries</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Roots of Wisdom</t>
+          <t>Ravenform</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Run Amok</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Run Ashore</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Runed Crown</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Rune of Flight</t>
+          <t>Reckless Crew</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Sarulf, Realm Eater</t>
+          <t>Reckless Crew</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Sarulf, Realm Eater</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Sarulf's Packmate</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Saw It Coming</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Sculptor of Winter</t>
+          <t>"Reidane, God of Justice" // "Reidane's Shield"</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Search for Glory</t>
+          <t>"Reidane, God of Justice" // "Reidane's Shield"</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Search for Glory</t>
+          <t>Renegade Reaper</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Seize the Spoils</t>
+          <t>Replicating Ring</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Shepherd of the Cosmos</t>
+          <t>"Resolute Valkyrie"</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>"Shirtless Snow Wizard"</t>
+          <t>Revitalize</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Showdown of the Skalds</t>
+          <t>Rimewood Falls</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Sigrid, God-Favored</t>
+          <t>Rise of the Dread Marn</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Sigrid, God-Favored</t>
+          <t>Rise of the Dread Marn</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Skemfar Shadowsage</t>
+          <t>Roots of Wisdom</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>"Ski Resort Bandit"</t>
+          <t>Run Amok</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Snakeskin Veil</t>
+          <t>Run Ashore</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Snow-Covered Forest</t>
+          <t>Runed Crown</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Snow-Covered Forest</t>
+          <t>Rune of Flight</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Snow-Covered Island</t>
+          <t>Sarulf, Realm Eater</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Snow-Covered Island</t>
+          <t>Sarulf, Realm Eater</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Snow-Covered Mountain</t>
+          <t>Sarulf's Packmate</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Snow-Covered Mountain</t>
+          <t>Saw It Coming</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Snow-Covered Plains</t>
+          <t>Scorn Effigy</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Snow-Covered Plains</t>
+          <t>Sculptor of Winter</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Snow-Covered Swamp</t>
+          <t>Search for Glory</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Snow-Covered Swamp</t>
+          <t>Search for Glory</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Snowfield Sinkhole</t>
+          <t>Seize the Spoils</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Spectral Steel</t>
+          <t>Shepherd of the Cosmos</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Spirit of the Aldergard</t>
+          <t>Showdown of the Skalds</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Squash</t>
+          <t>Sigrid, God-Favored</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Starnheim Aspirant</t>
+          <t>Sigrid, God-Favored</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Starnheim Unleashed</t>
+          <t>Skemfar Avenger</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Starnheim Unleashed</t>
+          <t>Skemfar Elderhall</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Sulfurous Mire</t>
+          <t>Skemfar Shadowsage</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Surtland Elementalist</t>
+          <t>Smashing Success</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Surtland Flinger</t>
+          <t>Snakeskin Veil</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Swamp</t>
+          <t>Snow-Covered Forest</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
+          <t>Snow-Covered Forest</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
+          <t>Snow-Covered Island</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Tergrid's Shadow</t>
+          <t>Snow-Covered Island</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>The Trickster-God's Heist</t>
+          <t>Snow-Covered Mountain</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>The World Tree</t>
+          <t>Snow-Covered Mountain</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Thornmantle Striker</t>
+          <t>Snow-Covered Plains</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Tibalt's Trickery</t>
+          <t>Snow-Covered Plains</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Tibalt's Trickery</t>
+          <t>Snow-Covered Swamp</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Toralf, God of Fury // Toralf's Hammer</t>
+          <t>Snow-Covered Swamp</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Toralf, God of Fury // Toralf's Hammer</t>
+          <t>Snowfield Sinkhole</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Tormentor's Helm</t>
+          <t>Spectral Steel</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Toski, Bearer of Secrets</t>
+          <t>Spirit of the Aldergard</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Toski, Bearer of Secrets</t>
+          <t>Squash</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Tyvar Kell</t>
+          <t>Starnheim Aspirant</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Tyvar Kell</t>
+          <t>Starnheim Unleashed</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Undersea Invader</t>
+          <t>Starnheim Unleashed</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>Strategic Planning</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>Sulfurous Mire</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>Surtland Elementalist</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Valkyrie Harbinger</t>
+          <t>Surtland Flinger</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Varragoth, Bloodsky Sire</t>
+          <t>"Surtland Frostfire"</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Varragoth, Bloodsky Sire</t>
+          <t>Swamp</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Vega, the Watcher</t>
+          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Vega, the Watcher</t>
+          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Village Rites</t>
+          <t>Tergrid's Shadow</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Volatile Fjord</t>
+          <t>The Bears of Littjara</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Vorinclex, Monstrous Raider</t>
+          <t>The Trickster-God's Heist</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Vorinclex, Monstrous Raider</t>
+          <t>The World Tree</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>|lornScs DuJhetmiserc.</t>
+          <t>Thornmantle Striker</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Waking the Trolls</t>
+          <t>Tibalt's Trickery</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Warchanter Skald</t>
+          <t>Tibalt's Trickery</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Weathered Runestone</t>
+          <t>Toralf, God of Fury // Toralf's Hammer</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Wings of the Cosmos</t>
+          <t>Toralf, God of Fury // Toralf's Hammer</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Withercrown</t>
+          <t>Tormentor's Helm</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Woodland Chasm</t>
+          <t>Toski, Bearer of Secrets</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
+        <is>
+          <t>Toski, Bearer of Secrets</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Tundra Fumarole</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Tundra Fumarole</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Tuskeri Firewalker</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Tyvar Kell</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Tyvar Kell</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Undersea Invader</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Usher of the Fallen</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Valkyrie Harbinger</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Varragoth, Bloodsky Sire</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Varragoth, Bloodsky Sire</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Vault Robber</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Vega, the Watcher</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Vega, the Watcher</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Village Rites</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Volatile Fjord</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Vorinclex, Monstrous Raider</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Vorinclex, Monstrous Raider</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>|lornScs DuJhetmiserc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Waking the Trolls</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Warchanter Skald</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Weathered Runestone</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Wings of the Cosmos</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Withercrown</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Woodland Chasm</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>"Writing Werewolf Fanfics"</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
         <is>
           <t>Youthful Valkyrie</t>
         </is>

</xml_diff>

<commit_message>
Update database upgraded using pickle
</commit_message>
<xml_diff>
--- a/Datos/Database by set/Set by name/Xlsx sets/Kaldheim (KHM).xlsx
+++ b/Datos/Database by set/Set by name/Xlsx sets/Kaldheim (KHM).xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A354"/>
+  <dimension ref="A1:A375"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -640,49 +640,49 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Battle of Frost and Fire</t>
+          <t>Battle Mammoth</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Bearded Axe</t>
+          <t>Battle Mammoth</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Behold the Multiverse</t>
+          <t>Battle of Frost and Fire</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Berg Strider</t>
+          <t>Bearded Axe</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Beskir Shieldmate</t>
+          <t>Behold the Multiverse</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>"Big Stabby"</t>
+          <t>Berg Strider</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>"Big Stabby"</t>
+          <t>Beskir Shieldmate</t>
         </is>
       </c>
     </row>
@@ -696,21 +696,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>"Birgi, God of Tales" // "Harnfel, Horn of Abundance"</t>
+          <t>Birgi, God of Storytelling // Harnfel, Horn of Bounty</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>"Birgi, God of Tales" // "Harnfel, Horn of Abundance"</t>
+          <t>Birgi, God of Storytelling // Harnfel, Horn of Bounty</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Blightstep Pathway // Searstep Pathway</t>
+          <t>Blessing of Frost</t>
         </is>
       </c>
     </row>
@@ -724,21 +724,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Blizzard Brawl</t>
+          <t>Blightstep Pathway // Searstep Pathway</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bloodline Pretender</t>
+          <t>Blizzard Brawl</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Blood on the Snow</t>
+          <t>Bloodline Pretender</t>
         </is>
       </c>
     </row>
@@ -752,2161 +752,2308 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Bloodsky Berserker</t>
+          <t>Blood on the Snow</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Boreal Outrider</t>
+          <t>Bloodsky Berserker</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Bound in Gold</t>
+          <t>Boreal Outrider</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Breakneck Berserker</t>
+          <t>Bound in Gold</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Bretagard Stronghold</t>
+          <t>Breakneck Berserker</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Broken Wings</t>
+          <t>Bretagard Stronghold</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Burning-Rune Demon</t>
+          <t>Brinebarrow Intruder</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Calamity Bearer</t>
+          <t>Broken Wings</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Calamity Bearer</t>
+          <t>Burning-Rune Demon</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Canopy Tactician</t>
+          <t>Burning-Rune Demon</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Cinderheart Giant</t>
+          <t>Calamity Bearer</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Clarion Spirit</t>
+          <t>Calamity Bearer</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Cleaving Reaper</t>
+          <t>Canopy Tactician</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Codespell Cleric</t>
+          <t>"Chill Out"</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Colossal Plow</t>
+          <t>Cinderheart Giant</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Cosima, God of the Voyage // The Omenkeel</t>
+          <t>Clarion Spirit</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Cosima, God of the Voyage // The Omenkeel</t>
+          <t>Cleaving Reaper</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Cosmos Charger</t>
+          <t>Codespell Cleric</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Cosmos Charger</t>
+          <t>Colossal Plow</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Cosmos Elixir</t>
+          <t>Cosima, God of the Voyage // The Omenkeel</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Crush the Weak</t>
+          <t>Cosima, God of the Voyage // The Omenkeel</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Cyclone Summoner</t>
+          <t>Cosmos Charger</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Cyclone Summoner</t>
+          <t>Cosmos Charger</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Darkbore Pathway // Slitherbore Pathway</t>
+          <t>Cosmos Elixir</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Darkbore Pathway // Slitherbore Pathway</t>
+          <t>Craven Hulk</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Deathknell Berserker</t>
+          <t>Crippling Fear</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Demon Bolt</t>
+          <t>Crush the Weak</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Demonic Gifts</t>
+          <t>Cyclone Summoner</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Disdainful Stroke</t>
+          <t>Cyclone Summoner</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Divine Gambit</t>
+          <t>Darkbore Pathway // Slitherbore Pathway</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Dogged Pursuit</t>
+          <t>Darkbore Pathway // Slitherbore Pathway</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Doomskar Oracle</t>
+          <t>Deathknell Berserker</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Doomskar Titan</t>
+          <t>Demon Bolt</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>"Dragon Dad uwu…"</t>
+          <t>Demonic Gifts</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Draugr Necromancer</t>
+          <t>Disdainful Stroke</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Draugr Necromancer</t>
+          <t>Divine Gambit</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Draugr's Helm</t>
+          <t>Dogged Pursuit</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Draugr Thought-Thief</t>
+          <t>Doomskar</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Dread Rider</t>
+          <t>Doomskar Oracle</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Dream Devourer</t>
+          <t>Doomskar Titan</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Dual Strike</t>
+          <t>Dragonkin Berserker</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Duskwielder</t>
+          <t>Dragonkin Berserker</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>"Dwarven Hammer"</t>
+          <t>Draugr Necromancer</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Dwarven Reinforcements</t>
+          <t>Draugr Necromancer</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Egon, God of Death // Throne of Death</t>
+          <t>Draugr's Helm</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Egon, God of Death // Throne of Death</t>
+          <t>Draugr Thought-Thief</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Elderfang Disciple</t>
+          <t>Dread Rider</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Elderfang Ritualist</t>
+          <t>Dream Devourer</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Elderleaf Mentor</t>
+          <t>Dual Strike</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Elven Ambush</t>
+          <t>Duskwielder</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Elvish Warmaster</t>
+          <t>Dwarven Hammer</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Elvish Warmaster</t>
+          <t>Dwarven Reinforcements</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Eradicator Valkyrie</t>
+          <t>Egon, God of Death // Throne of Death</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Eradicator Valkyrie</t>
+          <t>Egon, God of Death // Throne of Death</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Esika, God of the Tree // The Prismatic Bridge</t>
+          <t>Elderfang Disciple</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Esika, God of the Tree // The Prismatic Bridge</t>
+          <t>Elderfang Ritualist</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Esika's Chariot</t>
+          <t>Elderleaf Mentor</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Esika's Chariot</t>
+          <t>Elven Ambush</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Faceless Haven</t>
+          <t>Elvish Warmaster</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Faceless Haven</t>
+          <t>Elvish Warmaster</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Fall of the Impostor</t>
+          <t>Eradicator Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Fearless Liberator</t>
+          <t>Eradicator Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Fearless Pup</t>
+          <t>Esika, God of the Tree // The Prismatic Bridge</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Feed the Serpent</t>
+          <t>Esika, God of the Tree // The Prismatic Bridge</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Fire Giant's Fury</t>
+          <t>Esika's Chariot</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Firja, Judge of Valor</t>
+          <t>Esika's Chariot</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Firja, Judge of Valor</t>
+          <t>Faceless Haven</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Firja's Retribution</t>
+          <t>Faceless Haven</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Forest</t>
+          <t>Fall of the Impostor</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Forging the Tyrite Sword</t>
+          <t>"Family Get-Together"</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Frenzied Raider</t>
+          <t>"Family Get-Together"</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Frost Augur</t>
+          <t>Fearless Liberator</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Frost Bite</t>
+          <t>Fearless Pup</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Frost Bite</t>
+          <t>Feed the Serpent</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Frostpeak Yeti</t>
+          <t>Fire Giant's Fury</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Frostpyre Arcanist</t>
+          <t>Firja, Judge of Valor</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>"Frozen Blessing"</t>
+          <t>Firja, Judge of Valor</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Funeral Longboat</t>
+          <t>Firja's Retribution</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Fynn, the Fangbearer</t>
+          <t>Forest</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Gates of Istfell</t>
+          <t>Forging the Tyrite Sword</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Giant Ox</t>
+          <t>Frenzied Raider</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Giant's Amulet</t>
+          <t>Frost Augur</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Giant's Grasp</t>
+          <t>Frost Bite</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Gilded Assault Cart</t>
+          <t>Frost Bite</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Glacial Floodplain</t>
+          <t>Frostpeak Yeti</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Gladewalker Ritualist</t>
+          <t>Frostpyre Arcanist</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Glimpse the Cosmos</t>
+          <t>Funeral Longboat</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Glittering Frost</t>
+          <t>Fynn, the Fangbearer</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>"Glorious Protector"</t>
+          <t>Gates of Istfell</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>"Glorious Protector"</t>
+          <t>Giant Ox</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Gnottvold Recluse</t>
+          <t>Giant's Amulet</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Gnottvold Slumbermound</t>
+          <t>Giant's Grasp</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Gods' Hall Guardian</t>
+          <t>Gilded Assault Cart</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Goldmaw Champion</t>
+          <t>Glacial Floodplain</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Goldspan Dragon</t>
+          <t>Gladewalker Ritualist</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Goldspan Dragon</t>
+          <t>Glimpse the Cosmos</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Goldvein Pick</t>
+          <t>Glittering Frost</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Graven Lore</t>
+          <t>Glorious Protector</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Grim Draugr</t>
+          <t>Glorious Protector</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Guardian Gladewalker</t>
+          <t>Gnottvold Recluse</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Hagi Mob</t>
+          <t>Gnottvold Slumbermound</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Hailstorm Valkyrie</t>
+          <t>Gods' Hall Guardian</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Halvar, God of Battle // Sword of the Realms</t>
+          <t>Goldmaw Champion</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Halvar, God of Battle // Sword of the Realms</t>
+          <t>Goldspan Dragon</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Harald, King of Skemfar</t>
+          <t>Goldspan Dragon</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Harald, King of Skemfar</t>
+          <t>Goldvein Pick</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Harald Unites the Elves</t>
+          <t>Graven Lore</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Hengegate Pathway // Mistgate Pathway</t>
+          <t>Great Hall of Starnheim</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Hengegate Pathway // Mistgate Pathway</t>
+          <t>Grim Draugr</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Highland Forest</t>
+          <t>Grizzled Outrider</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Horizon Seeker</t>
+          <t>Guardian Gladewalker</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>"Horrible Encounter"</t>
+          <t>Hagi Mob</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Icehide Troll</t>
+          <t>Hailstorm Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Ice Tunnel</t>
+          <t>Halvar, God of Battle // Sword of the Realms</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Immersturm Predator</t>
+          <t>Halvar, God of Battle // Sword of the Realms</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Immersturm Predator</t>
+          <t>Harald, King of Skemfar</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Immersturm Raider</t>
+          <t>Harald, King of Skemfar</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Immersturm Skullcairn</t>
+          <t>Harald Unites the Elves</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Infernal Pet</t>
+          <t>Hengegate Pathway // Mistgate Pathway</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Inga Rune-Eyes</t>
+          <t>Hengegate Pathway // Mistgate Pathway</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Inga Rune-Eyes</t>
+          <t>Highland Forest</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>In Search of Greatness</t>
+          <t>Horizon Seeker</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Invasion of the Giants</t>
+          <t>Icehide Troll</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Iron Verdict</t>
+          <t>Ice Tunnel</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Island</t>
+          <t>Immersturm Predator</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Jarl of the Forsaken</t>
+          <t>Immersturm Predator</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Jaspera Sentinel</t>
+          <t>Immersturm Raider</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
+          <t>Immersturm Skullcairn</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
+          <t>Infernal Pet</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Kardur, Doomscourge</t>
+          <t>Inga Rune-Eyes</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Kardur, Doomscourge</t>
+          <t>Inga Rune-Eyes</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Kardur's Vicious Return</t>
+          <t>In Search of Greatness</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Karfell Harbinger</t>
+          <t>In Search of Greatness</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Karfell Kennel-Master</t>
+          <t>Invasion of the Giants</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Kaya's Onslaught</t>
+          <t>Invoke the Divine</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Kaya the Inexorable</t>
+          <t>Iron Verdict</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Kaya the Inexorable</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>King Harald's Revenge</t>
+          <t>Jarl of the Forsaken</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Koll, the Forgemaster</t>
+          <t>Jaspera Sentinel</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Koll, the Forgemaster</t>
+          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
+          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
+          <t>Kardur, Doomscourge</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Koma, Cosmos Serpent</t>
+          <t>Kardur, Doomscourge</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Koma, Cosmos Serpent</t>
+          <t>Kardur's Vicious Return</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Koma's Faithful</t>
+          <t>Karfell Harbinger</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Littjara Glade-Warden</t>
+          <t>Karfell Kennel-Master</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Littjara Kinseekers</t>
+          <t>Kaya's Onslaught</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Littjara Mirrorlake</t>
+          <t>Kaya the Inexorable</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Magda, Brazen Outlaw</t>
+          <t>Kaya the Inexorable</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Magda, Brazen Outlaw</t>
+          <t>King Harald's Revenge</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Maja, Bretagard Protector</t>
+          <t>"King Narfi's Betrayal"</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Mammoth Growth</t>
+          <t>Koll, the Forgemaster</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Masked Vandal</t>
+          <t>Koll, the Forgemaster</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Masked Vandal</t>
+          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Maskwood Nexus</t>
+          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Maskwood Nexus</t>
+          <t>Koma, Cosmos Serpent</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>"Master Skald"</t>
+          <t>Koma, Cosmos Serpent</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Moritte of the Frost</t>
+          <t>Koma's Faithful</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Mountain</t>
+          <t>Littjara Glade-Warden</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>"My D&amp;D OC"</t>
+          <t>Littjara Kinseekers</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Mystic Reflection</t>
+          <t>Littjara Mirrorlake</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Mystic Reflection</t>
+          <t>Magda, Brazen Outlaw</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Narfi, Betrayer King</t>
+          <t>Magda, Brazen Outlaw</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Narfi, Betrayer King</t>
+          <t>Maja, Bretagard Protector</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Niko Aris</t>
+          <t>Mammoth Growth</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Niko Aris</t>
+          <t>Masked Vandal</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Niko Defies Destiny</t>
+          <t>Masked Vandal</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Old-Growth Troll</t>
+          <t>Maskwood Nexus</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Old-Growth Troll</t>
+          <t>Maskwood Nexus</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Open the Omenpaths</t>
+          <t>Master Skald</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Path to the World Tree</t>
+          <t>Moritte of the Frost</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Pilfering Hawk</t>
+          <t>Mountain</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Plains</t>
+          <t>Mystic Reflection</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Poison the Cup</t>
+          <t>Mystic Reflection</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Poison the Cup</t>
+          <t>Narfi, Betrayer King</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Port of Karfell</t>
+          <t>Narfi, Betrayer King</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>"Priest of the Dam"</t>
+          <t>Niko Aris</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Provoke the Trolls</t>
+          <t>Niko Aris</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Pyre of Heroes</t>
+          <t>Niko Defies Destiny</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Pyre of Heroes</t>
+          <t>Old-Growth Troll</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Quakebringer</t>
+          <t>Old-Growth Troll</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Quakebringer</t>
+          <t>Open the Omenpaths</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Raiders' Karve</t>
+          <t>Orvar, the All-Form</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Raise the Draugr</t>
+          <t>Orvar, the All-Form</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Rally the Ranks</t>
+          <t>Path to the World Tree</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Rally the Ranks</t>
+          <t>Pilfering Hawk</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Rampage of the Valkyries</t>
+          <t>Plains</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Ravenform</t>
+          <t>Poison the Cup</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>"Ravenous Lindwurm"</t>
+          <t>Poison the Cup</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Raven Wings</t>
+          <t>Port of Karfell</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Priest of the Haunted Edge</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Provoke the Trolls</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Pyre of Heroes</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Reckless Crew</t>
+          <t>Pyre of Heroes</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Reckless Crew</t>
+          <t>Quakebringer</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Quakebringer</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Raiders' Karve</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Raise the Draugr</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Reidane, God of the Worthy // Valkmira, Protector's Shield</t>
+          <t>Rally the Ranks</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Reidane, God of the Worthy // Valkmira, Protector's Shield</t>
+          <t>Rally the Ranks</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Renegade Reaper</t>
+          <t>Rampage of the Valkyries</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Replicating Ring</t>
+          <t>Ravenform</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Return Upon the Tide</t>
+          <t>Ravenous Lindwurm</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Revitalize</t>
+          <t>Raven Wings</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Rimewood Falls</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Rise of the Dread Marn</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Rise of the Dread Marn</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Rootless Yew</t>
+          <t>Reckless Crew</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Roots of Wisdom</t>
+          <t>Reckless Crew</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Run Amok</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Run Ashore</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Runed Crown</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Rune of Flight</t>
+          <t>Reidane, God of the Worthy // Valkmira, Protector's Shield</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Sarulf, Realm Eater</t>
+          <t>Reidane, God of the Worthy // Valkmira, Protector's Shield</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Sarulf, Realm Eater</t>
+          <t>Renegade Reaper</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Sarulf's Packmate</t>
+          <t>Replicating Ring</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Saw It Coming</t>
+          <t>Resplendent Marshal</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Scorn Effigy</t>
+          <t>Return Upon the Tide</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Sculptor of Winter</t>
+          <t>Revitalize</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Search for Glory</t>
+          <t>Righteous Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Search for Glory</t>
+          <t>Rimewood Falls</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Seize the Spoils</t>
+          <t>Rise of the Dread Marn</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Shepherd of the Cosmos</t>
+          <t>Rise of the Dread Marn</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Showdown of the Skalds</t>
+          <t>Rootless Yew</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Sigrid, God-Favored</t>
+          <t>Roots of Wisdom</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Sigrid, God-Favored</t>
+          <t>Run Amok</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Skemfar Avenger</t>
+          <t>Run Ashore</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Skemfar Avenger</t>
+          <t>Runed Crown</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Skemfar Elderhall</t>
+          <t>Rune of Flight</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Skemfar Shadowsage</t>
+          <t>Sarulf, Realm Eater</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Skull Raid</t>
+          <t>Sarulf, Realm Eater</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Smashing Success</t>
+          <t>Sarulf's Packmate</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Snakeskin Veil</t>
+          <t>Saw It Coming</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Snow-Covered Forest</t>
+          <t>Scorn Effigy</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Snow-Covered Forest</t>
+          <t>Sculptor of Winter</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Snow-Covered Island</t>
+          <t>Search for Glory</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Snow-Covered Island</t>
+          <t>Search for Glory</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Snow-Covered Mountain</t>
+          <t>Seize the Spoils</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Snow-Covered Mountain</t>
+          <t>Shackles of Treachery</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Snow-Covered Plains</t>
+          <t>Shepherd of the Cosmos</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Snow-Covered Plains</t>
+          <t>Shimmerdrift Vale</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Snow-Covered Swamp</t>
+          <t>Showdown of the Skalds</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Snow-Covered Swamp</t>
+          <t>Sigrid, God-Favored</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Snowfield Sinkhole</t>
+          <t>Sigrid, God-Favored</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Spectral Steel</t>
+          <t>Skemfar Avenger</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Spirit of the Aldergard</t>
+          <t>Skemfar Avenger</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Squash</t>
+          <t>Skemfar Elderhall</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Stalwart Valkyrie</t>
+          <t>Skemfar Shadowsage</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Starnheim Aspirant</t>
+          <t>Skull Raid</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Starnheim Unleashed</t>
+          <t>Smashing Success</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Starnheim Unleashed</t>
+          <t>Snakeskin Veil</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Story Seeker</t>
+          <t>Snow-Covered Forest</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Strategic Planning</t>
+          <t>Snow-Covered Forest</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Strategic Planning</t>
+          <t>Snow-Covered Island</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>Sulfurous Mire</t>
+          <t>Snow-Covered Island</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>Surtland Elementalist</t>
+          <t>Snow-Covered Mountain</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Surtland Flinger</t>
+          <t>Snow-Covered Mountain</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>"Surtland Frostfire"</t>
+          <t>Snow-Covered Plains</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Svella, Ice Shaper</t>
+          <t>Snow-Covered Plains</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>Swamp</t>
+          <t>Snow-Covered Swamp</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
+          <t>Snow-Covered Swamp</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
+          <t>Snowfield Sinkhole</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>Tergrid's Shadow</t>
+          <t>Spectral Steel</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>The Bears of Littjara</t>
+          <t>Spirit of the Aldergard</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>The Bloodsky Massacre</t>
+          <t>Squash</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>The Raven's Warning</t>
+          <t>Stalwart Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>The Trickster-God's Heist</t>
+          <t>Starnheim Aspirant</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>The World Tree</t>
+          <t>Starnheim Courser</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Thornmantle Striker</t>
+          <t>Starnheim Unleashed</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Tibalt's Trickery</t>
+          <t>Starnheim Unleashed</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>Tibalt's Trickery</t>
+          <t>Story Seeker</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Toralf, God of Fury // Toralf's Hammer</t>
+          <t>Strategic Planning</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Toralf, God of Fury // Toralf's Hammer</t>
+          <t>Strategic Planning</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Tormentor's Helm</t>
+          <t>Sulfurous Mire</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Toski, Bearer of Secrets</t>
+          <t>Surtland Elementalist</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Toski, Bearer of Secrets</t>
+          <t>Surtland Flinger</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Tundra Fumarole</t>
+          <t>Surtland Frostpyre</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>Tundra Fumarole</t>
+          <t>Svella, Ice Shaper</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>Tuskeri Firewalker</t>
+          <t>Swamp</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>Tyrite Sanctum</t>
+          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>Tyvar Kell</t>
+          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>Tyvar Kell</t>
+          <t>Tergrid's Shadow</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>Undersea Invader</t>
+          <t>The Bears of Littjara</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>Usher of the Fallen</t>
+          <t>The Bloodsky Massacre</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>Usher of the Fallen</t>
+          <t>"The First Snowman"</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>The Raven's Warning</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>The Trickster-God's Heist</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>The World Tree</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Valkyrie Harbinger</t>
+          <t>Thornmantle Striker</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Valkyrie's Sword</t>
+          <t>Tibalt's Trickery</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>"Valley of Lights"</t>
+          <t>Tibalt's Trickery</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>Varragoth, Bloodsky Sire</t>
+          <t>Toralf, God of Fury // Toralf's Hammer</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>Varragoth, Bloodsky Sire</t>
+          <t>Toralf, God of Fury // Toralf's Hammer</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Vault Robber</t>
+          <t>Tormentor's Helm</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>Vega, the Watcher</t>
+          <t>Toski, Bearer of Secrets</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Vega, the Watcher</t>
+          <t>Toski, Bearer of Secrets</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Village Rites</t>
+          <t>Tundra Fumarole</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Volatile Fjord</t>
+          <t>Tundra Fumarole</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Vorinclex, Monstrous Raider</t>
+          <t>Tuskeri Firewalker</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>Vorinclex, Monstrous Raider</t>
+          <t>Tyrite Sanctum</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>|lornScs DuJhetmiserc.</t>
+          <t>Tyvar Kell</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Waking the Trolls</t>
+          <t>Tyvar Kell</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Warchanter Skald</t>
+          <t>Undersea Invader</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>"War Horn Blessing"</t>
+          <t>Usher of the Fallen</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>Weathered Runestone</t>
+          <t>Usher of the Fallen</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>Wings of the Cosmos</t>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>Withercrown</t>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>Woodland Chasm</t>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
+        <is>
+          <t>Valkyrie Harbinger</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>Valkyrie's Sword</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>Valor of the Worthy</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>Varragoth, Bloodsky Sire</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>Varragoth, Bloodsky Sire</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>Vault Robber</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>Vega, the Watcher</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>Vega, the Watcher</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>Village Rites</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>Volatile Fjord</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Vorinclex, Monstrous Raider</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>Vorinclex, Monstrous Raider</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>|lornScs DuJhetmiserc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>Waking the Trolls</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>Warchanter Skald</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>Warhorn Blast</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>Weathered Runestone</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>Weigh Down</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>Wings of the Cosmos</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>Withercrown</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>Woodland Chasm</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
         <is>
           <t>Youthful Valkyrie</t>
         </is>

</xml_diff>

<commit_message>
Added Deck statistics and card finder
</commit_message>
<xml_diff>
--- a/Datos/Database by set/Set by name/Xlsx sets/Kaldheim (KHM).xlsx
+++ b/Datos/Database by set/Set by name/Xlsx sets/Kaldheim (KHM).xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A375"/>
+  <dimension ref="A1:A406"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,14 +535,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Arni Slays the Troll</t>
+          <t>Arni Brokenbrow</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ascendant Spirit</t>
+          <t>Arni Slays the Troll</t>
         </is>
       </c>
     </row>
@@ -556,49 +556,49 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ascent of the Worthy</t>
+          <t>Ascendant Spirit</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Augury Raven</t>
+          <t>Ascent of the Worthy</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Avalanche Caller</t>
+          <t>Augury Raven</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Axgard Armory</t>
+          <t>Avalanche Caller</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Axgard Braggart</t>
+          <t>Axgard Armory</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Axgard Cavalry</t>
+          <t>Axgard Braggart</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Barkchannel Pathway // Tidechannel Pathway</t>
+          <t>Axgard Cavalry</t>
         </is>
       </c>
     </row>
@@ -612,35 +612,35 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Basalt Ravager</t>
+          <t>Barkchannel Pathway // Tidechannel Pathway</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Battershield Warrior</t>
+          <t>Basalt Ravager</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Battlefield Raptor</t>
+          <t>Battershield Warrior</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Battle for Bretagard</t>
+          <t>Battlefield Raptor</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Battle Mammoth</t>
+          <t>Battle for Bretagard</t>
         </is>
       </c>
     </row>
@@ -654,2406 +654,2623 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Battle of Frost and Fire</t>
+          <t>Battle Mammoth</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bearded Axe</t>
+          <t>Battle of Frost and Fire</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Behold the Multiverse</t>
+          <t>Bearded Axe</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Berg Strider</t>
+          <t>Behold the Multiverse</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Beskir Shieldmate</t>
+          <t>Berg Strider</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Binding the Old Gods</t>
+          <t>Beskir Shieldmate</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Birgi, God of Storytelling // Harnfel, Horn of Bounty</t>
+          <t>Binding the Old Gods</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Birgi, God of Storytelling // Harnfel, Horn of Bounty</t>
+          <t>Bind the Monster</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Blessing of Frost</t>
+          <t>Birgi, God of Storytelling // Harnfel, Horn of Bounty</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Blightstep Pathway // Searstep Pathway</t>
+          <t>Birgi, God of Storytelling // Harnfel, Horn of Bounty</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Blightstep Pathway // Searstep Pathway</t>
+          <t>Blessing of Frost</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Blizzard Brawl</t>
+          <t>Blessing of Frost</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Bloodline Pretender</t>
+          <t>Blightstep Pathway // Searstep Pathway</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Blood on the Snow</t>
+          <t>Blightstep Pathway // Searstep Pathway</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Blood on the Snow</t>
+          <t>Blizzard Brawl</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Bloodsky Berserker</t>
+          <t>Bloodline Pretender</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Boreal Outrider</t>
+          <t>Blood on the Snow</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Bound in Gold</t>
+          <t>Blood on the Snow</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Breakneck Berserker</t>
+          <t>Bloodsky Berserker</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Bretagard Stronghold</t>
+          <t>Boreal Outrider</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Brinebarrow Intruder</t>
+          <t>Bound in Gold</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Broken Wings</t>
+          <t>Breakneck Berserker</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Burning-Rune Demon</t>
+          <t>Bretagard Stronghold</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Burning-Rune Demon</t>
+          <t>Brinebarrow Intruder</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Calamity Bearer</t>
+          <t>Broken Wings</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Calamity Bearer</t>
+          <t>Burning-Rune Demon</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Canopy Tactician</t>
+          <t>Burning-Rune Demon</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>"Chill Out"</t>
+          <t>Calamity Bearer</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Cinderheart Giant</t>
+          <t>Calamity Bearer</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Clarion Spirit</t>
+          <t>Canopy Tactician</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Cleaving Reaper</t>
+          <t>Cinderheart Giant</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Codespell Cleric</t>
+          <t>Clarion Spirit</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Colossal Plow</t>
+          <t>Cleaving Reaper</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Cosima, God of the Voyage // The Omenkeel</t>
+          <t>Codespell Cleric</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Cosima, God of the Voyage // The Omenkeel</t>
+          <t>Colossal Plow</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Cosmos Charger</t>
+          <t>Cosima, God of the Voyage // The Omenkeel</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Cosmos Charger</t>
+          <t>Cosima, God of the Voyage // The Omenkeel</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Cosmos Elixir</t>
+          <t>Cosmos Charger</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Craven Hulk</t>
+          <t>Cosmos Charger</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Crippling Fear</t>
+          <t>Cosmos Elixir</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Crush the Weak</t>
+          <t>Cosmos Elixir</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Cyclone Summoner</t>
+          <t>Craven Hulk</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Cyclone Summoner</t>
+          <t>Crippling Fear</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Darkbore Pathway // Slitherbore Pathway</t>
+          <t>Crippling Fear</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Darkbore Pathway // Slitherbore Pathway</t>
+          <t>Crush the Weak</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Deathknell Berserker</t>
+          <t>Cyclone Summoner</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Demon Bolt</t>
+          <t>Cyclone Summoner</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Demonic Gifts</t>
+          <t>Darkbore Pathway // Slitherbore Pathway</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Disdainful Stroke</t>
+          <t>Darkbore Pathway // Slitherbore Pathway</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Divine Gambit</t>
+          <t>Deathknell Berserker</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Dogged Pursuit</t>
+          <t>Demon Bolt</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Doomskar</t>
+          <t>Demonic Gifts</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Doomskar Oracle</t>
+          <t>Depart the Realm</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Doomskar Titan</t>
+          <t>Disdainful Stroke</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Dragonkin Berserker</t>
+          <t>Divine Gambit</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Dragonkin Berserker</t>
+          <t>Dogged Pursuit</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Draugr Necromancer</t>
+          <t>Doomskar</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Draugr Necromancer</t>
+          <t>Doomskar</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Draugr's Helm</t>
+          <t>Doomskar Oracle</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Draugr Thought-Thief</t>
+          <t>Doomskar Titan</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Dread Rider</t>
+          <t>Dragonkin Berserker</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Dream Devourer</t>
+          <t>Dragonkin Berserker</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Dual Strike</t>
+          <t>Draugr Necromancer</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Duskwielder</t>
+          <t>Draugr Necromancer</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Dwarven Hammer</t>
+          <t>Draugr Recruiter</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Dwarven Reinforcements</t>
+          <t>Draugr's Helm</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Egon, God of Death // Throne of Death</t>
+          <t>Draugr Thought-Thief</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Egon, God of Death // Throne of Death</t>
+          <t>Dread Rider</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Elderfang Disciple</t>
+          <t>Dream Devourer</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Elderfang Ritualist</t>
+          <t>Dream Devourer</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Elderleaf Mentor</t>
+          <t>Dual Strike</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Elven Ambush</t>
+          <t>Duskwielder</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Elvish Warmaster</t>
+          <t>Dwarven Hammer</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Elvish Warmaster</t>
+          <t>Dwarven Reinforcements</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Eradicator Valkyrie</t>
+          <t>Egon, God of Death // Throne of Death</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Eradicator Valkyrie</t>
+          <t>Egon, God of Death // Throne of Death</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Esika, God of the Tree // The Prismatic Bridge</t>
+          <t>Elderfang Disciple</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Esika, God of the Tree // The Prismatic Bridge</t>
+          <t>Elderfang Ritualist</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Esika's Chariot</t>
+          <t>Elderleaf Mentor</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Esika's Chariot</t>
+          <t>Elven Ambush</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Faceless Haven</t>
+          <t>Elven Bow</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Faceless Haven</t>
+          <t>Elvish Warmaster</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Fall of the Impostor</t>
+          <t>Elvish Warmaster</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>"Family Get-Together"</t>
+          <t>Eradicator Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>"Family Get-Together"</t>
+          <t>Eradicator Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Fearless Liberator</t>
+          <t>Esika, God of the Tree // The Prismatic Bridge</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Fearless Pup</t>
+          <t>Esika, God of the Tree // The Prismatic Bridge</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Feed the Serpent</t>
+          <t>Esika's Chariot</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Fire Giant's Fury</t>
+          <t>Esika's Chariot</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Firja, Judge of Valor</t>
+          <t>Faceless Haven</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Firja, Judge of Valor</t>
+          <t>Faceless Haven</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Firja's Retribution</t>
+          <t>Fall of the Impostor</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Forest</t>
+          <t>Fearless Liberator</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Forging the Tyrite Sword</t>
+          <t>Fearless Pup</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Frenzied Raider</t>
+          <t>Feed the Serpent</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Frost Augur</t>
+          <t>Fire Giant's Fury</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Frost Bite</t>
+          <t>Firja, Judge of Valor</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Frost Bite</t>
+          <t>Firja, Judge of Valor</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Frostpeak Yeti</t>
+          <t>Firja's Retribution</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Frostpyre Arcanist</t>
+          <t>Forest</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Funeral Longboat</t>
+          <t>Forging the Tyrite Sword</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Fynn, the Fangbearer</t>
+          <t>Frenzied Raider</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Gates of Istfell</t>
+          <t>Frost Augur</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Giant Ox</t>
+          <t>Frost Bite</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Giant's Amulet</t>
+          <t>Frost Bite</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Giant's Grasp</t>
+          <t>Frostpeak Yeti</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Gilded Assault Cart</t>
+          <t>Frostpyre Arcanist</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Glacial Floodplain</t>
+          <t>Funeral Longboat</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Gladewalker Ritualist</t>
+          <t>Fynn, the Fangbearer</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Glimpse the Cosmos</t>
+          <t>Fynn, the Fangbearer</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Glittering Frost</t>
+          <t>Gates of Istfell</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Glorious Protector</t>
+          <t>Giant Ox</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Glorious Protector</t>
+          <t>Giant's Amulet</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Gnottvold Recluse</t>
+          <t>Giant's Grasp</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Gnottvold Slumbermound</t>
+          <t>Gilded Assault Cart</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Gods' Hall Guardian</t>
+          <t>Glacial Floodplain</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Goldmaw Champion</t>
+          <t>Gladewalker Ritualist</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Goldspan Dragon</t>
+          <t>Glimpse the Cosmos</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Goldspan Dragon</t>
+          <t>Glittering Frost</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Goldvein Pick</t>
+          <t>Glorious Protector</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Graven Lore</t>
+          <t>Glorious Protector</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Great Hall of Starnheim</t>
+          <t>Gnottvold Recluse</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Grim Draugr</t>
+          <t>Gnottvold Slumbermound</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Grizzled Outrider</t>
+          <t>Gods' Hall Guardian</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Guardian Gladewalker</t>
+          <t>Goldmaw Champion</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Hagi Mob</t>
+          <t>Goldspan Dragon</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Hailstorm Valkyrie</t>
+          <t>Goldspan Dragon</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Halvar, God of Battle // Sword of the Realms</t>
+          <t>Goldvein Pick</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Halvar, God of Battle // Sword of the Realms</t>
+          <t>Graven Lore</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Harald, King of Skemfar</t>
+          <t>Graven Lore</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Harald, King of Skemfar</t>
+          <t>Great Hall of Starnheim</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Harald Unites the Elves</t>
+          <t>Grim Draugr</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Hengegate Pathway // Mistgate Pathway</t>
+          <t>Grizzled Outrider</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Hengegate Pathway // Mistgate Pathway</t>
+          <t>Guardian Gladewalker</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Highland Forest</t>
+          <t>Hagi Mob</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Horizon Seeker</t>
+          <t>Hailstorm Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Icehide Troll</t>
+          <t>Halvar, God of Battle // Sword of the Realms</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Ice Tunnel</t>
+          <t>Halvar, God of Battle // Sword of the Realms</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Immersturm Predator</t>
+          <t>Harald, King of Skemfar</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Immersturm Predator</t>
+          <t>Harald, King of Skemfar</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Immersturm Raider</t>
+          <t>Harald Unites the Elves</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Immersturm Skullcairn</t>
+          <t>Haunting Voyage</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Infernal Pet</t>
+          <t>Haunting Voyage</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Inga Rune-Eyes</t>
+          <t>Hengegate Pathway // Mistgate Pathway</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Inga Rune-Eyes</t>
+          <t>Hengegate Pathway // Mistgate Pathway</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>In Search of Greatness</t>
+          <t>Highland Forest</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>In Search of Greatness</t>
+          <t>Horizon Seeker</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Invasion of the Giants</t>
+          <t>Icebind Pillar</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Invoke the Divine</t>
+          <t>Icebreaker Kraken</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Iron Verdict</t>
+          <t>Icebreaker Kraken</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Island</t>
+          <t>Icehide Troll</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Jarl of the Forsaken</t>
+          <t>Ice Tunnel</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Jaspera Sentinel</t>
+          <t>Immersturm Predator</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
+          <t>Immersturm Predator</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
+          <t>Immersturm Raider</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Kardur, Doomscourge</t>
+          <t>Immersturm Skullcairn</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Kardur, Doomscourge</t>
+          <t>Infernal Pet</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Kardur's Vicious Return</t>
+          <t>Inga Rune-Eyes</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Karfell Harbinger</t>
+          <t>Inga Rune-Eyes</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Karfell Kennel-Master</t>
+          <t>In Search of Greatness</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Kaya's Onslaught</t>
+          <t>In Search of Greatness</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Kaya the Inexorable</t>
+          <t>Invasion of the Giants</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Kaya the Inexorable</t>
+          <t>Invoke the Divine</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>King Harald's Revenge</t>
+          <t>Iron Verdict</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>"King Narfi's Betrayal"</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Koll, the Forgemaster</t>
+          <t>Jarl of the Forsaken</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Koll, the Forgemaster</t>
+          <t>Jaspera Sentinel</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
+          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
+          <t>Jorn, God of Winter // Kaldring, the Rimestaff</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Koma, Cosmos Serpent</t>
+          <t>Kardur, Doomscourge</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Koma, Cosmos Serpent</t>
+          <t>Kardur, Doomscourge</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Koma's Faithful</t>
+          <t>Kardur's Vicious Return</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Littjara Glade-Warden</t>
+          <t>Karfell Harbinger</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Littjara Kinseekers</t>
+          <t>Karfell Kennel-Master</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Littjara Mirrorlake</t>
+          <t>Kaya's Onslaught</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Magda, Brazen Outlaw</t>
+          <t>Kaya the Inexorable</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Magda, Brazen Outlaw</t>
+          <t>Kaya the Inexorable</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Maja, Bretagard Protector</t>
+          <t>King Harald's Revenge</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Mammoth Growth</t>
+          <t>King Narfi's Betrayal</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Masked Vandal</t>
+          <t>Koll, the Forgemaster</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Masked Vandal</t>
+          <t>Koll, the Forgemaster</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Maskwood Nexus</t>
+          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Maskwood Nexus</t>
+          <t>Kolvori, God of Kinship // The Ringhart Crest</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Master Skald</t>
+          <t>Koma, Cosmos Serpent</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Moritte of the Frost</t>
+          <t>Koma, Cosmos Serpent</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Mountain</t>
+          <t>Koma's Faithful</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Mystic Reflection</t>
+          <t>Littjara Glade-Warden</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Mystic Reflection</t>
+          <t>Littjara Kinseekers</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Narfi, Betrayer King</t>
+          <t>Littjara Mirrorlake</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Narfi, Betrayer King</t>
+          <t>Magda, Brazen Outlaw</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Niko Aris</t>
+          <t>Magda, Brazen Outlaw</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Niko Aris</t>
+          <t>Maja, Bretagard Protector</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Niko Defies Destiny</t>
+          <t>Maja, Bretagard Protector</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Old-Growth Troll</t>
+          <t>Mammoth Growth</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Old-Growth Troll</t>
+          <t>Masked Vandal</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Open the Omenpaths</t>
+          <t>Masked Vandal</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Orvar, the All-Form</t>
+          <t>Maskwood Nexus</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Orvar, the All-Form</t>
+          <t>Maskwood Nexus</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Path to the World Tree</t>
+          <t>Master Skald</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Pilfering Hawk</t>
+          <t>Mists of Littjara</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Plains</t>
+          <t>Mistwalker</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Poison the Cup</t>
+          <t>Moritte of the Frost</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Poison the Cup</t>
+          <t>Moritte of the Frost</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Port of Karfell</t>
+          <t>Mountain</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Priest of the Haunted Edge</t>
+          <t>Mystic Reflection</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Provoke the Trolls</t>
+          <t>Mystic Reflection</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Pyre of Heroes</t>
+          <t>Narfi, Betrayer King</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Pyre of Heroes</t>
+          <t>Narfi, Betrayer King</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Quakebringer</t>
+          <t>Niko Aris</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Quakebringer</t>
+          <t>Niko Aris</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Raiders' Karve</t>
+          <t>Niko Defies Destiny</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Raise the Draugr</t>
+          <t>Old-Growth Troll</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Rally the Ranks</t>
+          <t>Old-Growth Troll</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Rally the Ranks</t>
+          <t>Open the Omenpaths</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Rampage of the Valkyries</t>
+          <t>Orvar, the All-Form</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Ravenform</t>
+          <t>Orvar, the All-Form</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Ravenous Lindwurm</t>
+          <t>Path to the World Tree</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Raven Wings</t>
+          <t>Pilfering Hawk</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Plains</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Poison the Cup</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Realmwalker</t>
+          <t>Poison the Cup</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Reckless Crew</t>
+          <t>Port of Karfell</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Reckless Crew</t>
+          <t>Priest of the Haunted Edge</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Provoke the Trolls</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Pyre of Heroes</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Reflections of Littjara</t>
+          <t>Pyre of Heroes</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Reidane, God of the Worthy // Valkmira, Protector's Shield</t>
+          <t>Quakebringer</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Reidane, God of the Worthy // Valkmira, Protector's Shield</t>
+          <t>Quakebringer</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Renegade Reaper</t>
+          <t>Raiders' Karve</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Replicating Ring</t>
+          <t>Raise the Draugr</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Resplendent Marshal</t>
+          <t>Rally the Ranks</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Return Upon the Tide</t>
+          <t>Rally the Ranks</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Revitalize</t>
+          <t>Rampage of the Valkyries</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Righteous Valkyrie</t>
+          <t>Ravenform</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Rimewood Falls</t>
+          <t>Ravenous Lindwurm</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Rise of the Dread Marn</t>
+          <t>Raven Wings</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Rise of the Dread Marn</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Rootless Yew</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Roots of Wisdom</t>
+          <t>Realmwalker</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Run Amok</t>
+          <t>Reckless Crew</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Run Ashore</t>
+          <t>Reckless Crew</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Runed Crown</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Rune of Flight</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Sarulf, Realm Eater</t>
+          <t>Reflections of Littjara</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Sarulf, Realm Eater</t>
+          <t>Reidane, God of the Worthy // Valkmira, Protector's Shield</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Sarulf's Packmate</t>
+          <t>Reidane, God of the Worthy // Valkmira, Protector's Shield</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Saw It Coming</t>
+          <t>Renegade Reaper</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Scorn Effigy</t>
+          <t>Replicating Ring</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Sculptor of Winter</t>
+          <t>Resplendent Marshal</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Search for Glory</t>
+          <t>Resplendent Marshal</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Search for Glory</t>
+          <t>Return Upon the Tide</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Seize the Spoils</t>
+          <t>Revitalize</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Shackles of Treachery</t>
+          <t>Righteous Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Shepherd of the Cosmos</t>
+          <t>Righteous Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Shimmerdrift Vale</t>
+          <t>Rimewood Falls</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Showdown of the Skalds</t>
+          <t>Rise of the Dread Marn</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Sigrid, God-Favored</t>
+          <t>Rise of the Dread Marn</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Sigrid, God-Favored</t>
+          <t>Rootless Yew</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Skemfar Avenger</t>
+          <t>Roots of Wisdom</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Skemfar Avenger</t>
+          <t>Run Amok</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Skemfar Elderhall</t>
+          <t>Run Ashore</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Skemfar Shadowsage</t>
+          <t>Runed Crown</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Skull Raid</t>
+          <t>Runeforge Champion</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Smashing Success</t>
+          <t>Runeforge Champion</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Snakeskin Veil</t>
+          <t>Rune of Flight</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Snow-Covered Forest</t>
+          <t>Rune of Might</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Snow-Covered Forest</t>
+          <t>Rune of Mortality</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Snow-Covered Island</t>
+          <t>Rune of Speed</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>Snow-Covered Island</t>
+          <t>Rune of Sustenance</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>Snow-Covered Mountain</t>
+          <t>Sarulf, Realm Eater</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Snow-Covered Mountain</t>
+          <t>Sarulf, Realm Eater</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>Snow-Covered Plains</t>
+          <t>Sarulf's Packmate</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Snow-Covered Plains</t>
+          <t>Saw It Coming</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>Snow-Covered Swamp</t>
+          <t>Scorn Effigy</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Snow-Covered Swamp</t>
+          <t>Sculptor of Winter</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Snowfield Sinkhole</t>
+          <t>Search for Glory</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>Spectral Steel</t>
+          <t>Search for Glory</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Spirit of the Aldergard</t>
+          <t>Seize the Spoils</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Squash</t>
+          <t>Shackles of Treachery</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>Stalwart Valkyrie</t>
+          <t>Shepherd of the Cosmos</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Starnheim Aspirant</t>
+          <t>Shimmerdrift Vale</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Starnheim Courser</t>
+          <t>Showdown of the Skalds</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Starnheim Unleashed</t>
+          <t>Sigrid, God-Favored</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Starnheim Unleashed</t>
+          <t>Sigrid, God-Favored</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>Story Seeker</t>
+          <t>Skemfar Avenger</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Strategic Planning</t>
+          <t>Skemfar Avenger</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Strategic Planning</t>
+          <t>Skemfar Elderhall</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Sulfurous Mire</t>
+          <t>Skemfar Shadowsage</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Surtland Elementalist</t>
+          <t>Skull Raid</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Surtland Flinger</t>
+          <t>Smashing Success</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Surtland Frostpyre</t>
+          <t>Snakeskin Veil</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>Svella, Ice Shaper</t>
+          <t>Snow-Covered Forest</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>Swamp</t>
+          <t>Snow-Covered Forest</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
+          <t>Snow-Covered Island</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
+          <t>Snow-Covered Island</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>Tergrid's Shadow</t>
+          <t>Snow-Covered Mountain</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>The Bears of Littjara</t>
+          <t>Snow-Covered Mountain</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>The Bloodsky Massacre</t>
+          <t>Snow-Covered Plains</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>"The First Snowman"</t>
+          <t>Snow-Covered Plains</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>The Raven's Warning</t>
+          <t>Snow-Covered Swamp</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>The Trickster-God's Heist</t>
+          <t>Snow-Covered Swamp</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>The World Tree</t>
+          <t>Snowfield Sinkhole</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Thornmantle Striker</t>
+          <t>Spectral Steel</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Tibalt's Trickery</t>
+          <t>Spirit of the Aldergard</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Tibalt's Trickery</t>
+          <t>Squash</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>Toralf, God of Fury // Toralf's Hammer</t>
+          <t>Stalwart Valkyrie</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>Toralf, God of Fury // Toralf's Hammer</t>
+          <t>Starnheim Aspirant</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Tormentor's Helm</t>
+          <t>Starnheim Courser</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>Toski, Bearer of Secrets</t>
+          <t>Starnheim Unleashed</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Toski, Bearer of Secrets</t>
+          <t>Starnheim Unleashed</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Tundra Fumarole</t>
+          <t>Story Seeker</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Tundra Fumarole</t>
+          <t>Strategic Planning</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Tuskeri Firewalker</t>
+          <t>Strategic Planning</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>Tyrite Sanctum</t>
+          <t>Struggle for Skemfar</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>Tyvar Kell</t>
+          <t>Sulfurous Mire</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Tyvar Kell</t>
+          <t>Surtland Elementalist</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Undersea Invader</t>
+          <t>Surtland Flinger</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Usher of the Fallen</t>
+          <t>Surtland Frostpyre</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>Usher of the Fallen</t>
+          <t>Svella, Ice Shaper</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>Svella, Ice Shaper</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>Swamp</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>Valkyrie Harbinger</t>
+          <t>Tergrid, God of Fright // Tergrid's Lantern</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>Valkyrie's Sword</t>
+          <t>Tergrid's Shadow</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>Valor of the Worthy</t>
+          <t>The Bears of Littjara</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>Varragoth, Bloodsky Sire</t>
+          <t>The Bloodsky Massacre</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>Varragoth, Bloodsky Sire</t>
+          <t>The Raven's Warning</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>Vault Robber</t>
+          <t>The Three Seasons</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>Vega, the Watcher</t>
+          <t>The Trickster-God's Heist</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>Vega, the Watcher</t>
+          <t>The World Tree</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>Village Rites</t>
+          <t>The World Tree</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>Volatile Fjord</t>
+          <t>Thornmantle Striker</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>Vorinclex, Monstrous Raider</t>
+          <t>Tibalt's Trickery</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>Vorinclex, Monstrous Raider</t>
+          <t>Tibalt's Trickery</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>|lornScs DuJhetmiserc.</t>
+          <t>Toralf, God of Fury // Toralf's Hammer</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>Waking the Trolls</t>
+          <t>Toralf, God of Fury // Toralf's Hammer</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>Warchanter Skald</t>
+          <t>Tormentor's Helm</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>Warhorn Blast</t>
+          <t>Toski, Bearer of Secrets</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>Weathered Runestone</t>
+          <t>Toski, Bearer of Secrets</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>Weigh Down</t>
+          <t>Tundra Fumarole</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>Wings of the Cosmos</t>
+          <t>Tundra Fumarole</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>Withercrown</t>
+          <t>Tuskeri Firewalker</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>Woodland Chasm</t>
+          <t>Tyrite Sanctum</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
+        <is>
+          <t>Tyrite Sanctum</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>Tyvar Kell</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>Tyvar Kell</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>Undersea Invader</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>Usher of the Fallen</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Usher of the Fallen</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>Valki, God of Lies // Tibalt, Cosmic Impostor</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>Valkyrie Harbinger</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>Valkyrie's Sword</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>Valor of the Worthy</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>Varragoth, Bloodsky Sire</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>Varragoth, Bloodsky Sire</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>Vault Robber</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>Vega, the Watcher</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>Vega, the Watcher</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>Vengeful Reaper</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>Village Rites</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>Volatile Fjord</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>Vorinclex, Monstrous Raider</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>Vorinclex, Monstrous Raider</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>|lornScs DuJhetmiserc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>Waking the Trolls</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>Warchanter Skald</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>Warhorn Blast</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>Weathered Runestone</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>Weigh Down</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>Wings of the Cosmos</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>Withercrown</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>Woodland Chasm</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
         <is>
           <t>Youthful Valkyrie</t>
         </is>

</xml_diff>